<commit_message>
report on stat of the art. Modified evaluation
</commit_message>
<xml_diff>
--- a/doc/visuDNA_comparaison_outils_de graphe.xlsx
+++ b/doc/visuDNA_comparaison_outils_de graphe.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastien_R\Documents\heia-2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Users\SebastienB\Personnal\heia-2017\visuDNA-ii\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Gephi</t>
   </si>
@@ -86,14 +86,14 @@
     <t>Version Java applet (seems complicated &amp; java desktop</t>
   </si>
   <si>
-    <t>Not open source</t>
+    <t>Pas d'annoation sur les nœuds/edges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,8 +109,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,26 +139,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39994506668294322"/>
+        <fgColor theme="5" tint="-0.24994659260841701"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.24994659260841701"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.24994659260841701"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -423,10 +429,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -463,30 +471,29 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -802,17 +809,20 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="10" max="10" width="28.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" style="26"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -847,7 +857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
@@ -878,7 +888,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="22"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
@@ -907,12 +917,12 @@
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="25">
+      <c r="K3" s="31">
         <f>SUMPRODUCT(B3:I3, $B$2:$I$2)</f>
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -935,54 +945,54 @@
         <v>2</v>
       </c>
       <c r="H4" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="7">
         <v>3</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="24">
+      <c r="K4" s="31">
         <f t="shared" ref="K4:K8" si="0">SUMPRODUCT(B4:I4, $B$2:$I$2)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="28">
-        <v>1</v>
-      </c>
-      <c r="C5" s="29">
-        <v>3</v>
-      </c>
-      <c r="D5" s="29">
-        <v>1</v>
-      </c>
-      <c r="E5" s="29">
-        <v>2</v>
-      </c>
-      <c r="F5" s="29">
-        <v>2</v>
-      </c>
-      <c r="G5" s="29">
-        <v>3</v>
-      </c>
-      <c r="H5" s="29">
-        <v>4</v>
-      </c>
-      <c r="I5" s="29">
-        <v>4</v>
-      </c>
-      <c r="J5" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="26">
+        <v>3</v>
+      </c>
+      <c r="C5" s="27">
+        <v>2</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1</v>
+      </c>
+      <c r="E5" s="27">
+        <v>2</v>
+      </c>
+      <c r="F5" s="27">
+        <v>2</v>
+      </c>
+      <c r="G5" s="27">
+        <v>3</v>
+      </c>
+      <c r="H5" s="27">
+        <v>4</v>
+      </c>
+      <c r="I5" s="27">
+        <v>4</v>
+      </c>
+      <c r="J5" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="31">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K5" s="29">
+        <f>SUMPRODUCT(B5:I5, $B$2:$I$2)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1005,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6" s="7">
         <v>3</v>
@@ -1013,46 +1023,46 @@
       <c r="J6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="23">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="17">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7">
-        <v>4</v>
-      </c>
-      <c r="E7" s="7">
-        <v>3</v>
-      </c>
-      <c r="F7" s="7">
-        <v>3</v>
-      </c>
-      <c r="G7" s="7">
-        <v>3</v>
-      </c>
-      <c r="H7" s="7">
-        <v>3</v>
-      </c>
-      <c r="I7" s="7">
-        <v>4</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="25">
+      <c r="K6" s="31">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>3</v>
+      </c>
+      <c r="H7" s="7">
+        <v>3</v>
+      </c>
+      <c r="I7" s="7">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="31">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1088,7 +1098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1098,7 +1108,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
@@ -1133,7 +1143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>16</v>
       </c>
@@ -1164,7 +1174,7 @@
       <c r="J11" s="12"/>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>0</v>
       </c>
@@ -1190,15 +1200,15 @@
         <v>4</v>
       </c>
       <c r="I12" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J12" s="1"/>
-      <c r="K12" s="25">
+      <c r="K12" s="31">
         <f>SUMPRODUCT(B12:I12, $B$11:$I$11)</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1206,7 +1216,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="7">
         <v>3</v>
@@ -1221,54 +1231,52 @@
         <v>3</v>
       </c>
       <c r="H13" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I13" s="7">
+        <v>4</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="31">
+        <f t="shared" ref="K13:K17" si="1">SUMPRODUCT(B13:I13, $B$11:$I$11)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="26">
+        <v>4</v>
+      </c>
+      <c r="C14" s="27">
+        <v>2</v>
+      </c>
+      <c r="D14" s="27">
+        <v>1</v>
+      </c>
+      <c r="E14" s="27">
+        <v>1</v>
+      </c>
+      <c r="F14" s="27">
+        <v>2</v>
+      </c>
+      <c r="G14" s="27">
+        <v>3</v>
+      </c>
+      <c r="H14" s="27">
+        <v>5</v>
+      </c>
+      <c r="I14" s="27">
         <v>6</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="24">
-        <f t="shared" ref="K13:K17" si="1">SUMPRODUCT(B13:I13, $B$11:$I$11)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="28">
-        <v>1</v>
-      </c>
-      <c r="C14" s="29">
-        <v>3</v>
-      </c>
-      <c r="D14" s="29">
-        <v>1</v>
-      </c>
-      <c r="E14" s="29">
-        <v>1</v>
-      </c>
-      <c r="F14" s="29">
-        <v>3</v>
-      </c>
-      <c r="G14" s="29">
-        <v>3</v>
-      </c>
-      <c r="H14" s="29">
-        <v>5</v>
-      </c>
-      <c r="I14" s="29">
-        <v>6</v>
-      </c>
-      <c r="J14" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="31">
+      <c r="J14" s="28"/>
+      <c r="K14" s="29">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -1288,7 +1296,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H15" s="7">
         <v>6</v>
@@ -1301,15 +1309,15 @@
       </c>
       <c r="K15" s="32">
         <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="7">
         <v>4</v>
@@ -1333,12 +1341,12 @@
         <v>5</v>
       </c>
       <c r="J16" s="2"/>
-      <c r="K16" s="33">
+      <c r="K16" s="31">
         <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1369,7 +1377,7 @@
       <c r="J17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="32">
+      <c r="K17" s="30">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
continued comparison file for Cyto., CSAT & Tulip
</commit_message>
<xml_diff>
--- a/doc/visuDNA_comparaison_outils_de graphe.xlsx
+++ b/doc/visuDNA_comparaison_outils_de graphe.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Notation1" sheetId="1" r:id="rId1"/>
-    <sheet name="Notation2" sheetId="2" r:id="rId2"/>
+    <sheet name="Formats" sheetId="3" r:id="rId2"/>
+    <sheet name="Notation2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="49">
   <si>
     <t>Gephi</t>
   </si>
@@ -99,13 +100,79 @@
     <t>CSAT</t>
   </si>
   <si>
-    <t>Supported input format</t>
-  </si>
-  <si>
-    <t>Language used for API</t>
-  </si>
-  <si>
-    <t>API quality</t>
+    <t>Formats</t>
+  </si>
+  <si>
+    <t>SIF</t>
+  </si>
+  <si>
+    <t>NNF</t>
+  </si>
+  <si>
+    <t>GML</t>
+  </si>
+  <si>
+    <t>XGMML</t>
+  </si>
+  <si>
+    <t>SBML</t>
+  </si>
+  <si>
+    <t>BioPAX</t>
+  </si>
+  <si>
+    <t>GraphML</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>XLS,XLSX</t>
+  </si>
+  <si>
+    <t>Cytoscape.js JSON</t>
+  </si>
+  <si>
+    <t>Node annotations</t>
+  </si>
+  <si>
+    <t>Edge annotation</t>
+  </si>
+  <si>
+    <t>Layout information</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>PSI-MI Level</t>
+  </si>
+  <si>
+    <t>TLP</t>
+  </si>
+  <si>
+    <t>GEXF (Gephi)</t>
+  </si>
+  <si>
+    <t>Matrice d'adjacence</t>
+  </si>
+  <si>
+    <t>Langages</t>
+  </si>
+  <si>
+    <t>Langage</t>
+  </si>
+  <si>
+    <t>Non défini</t>
+  </si>
+  <si>
+    <t>c++/python</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -173,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -484,6 +551,176 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -494,7 +731,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -566,6 +803,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -883,14 +1156,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
@@ -899,7 +1174,7 @@
     <col min="11" max="11" width="11.5703125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -934,7 +1209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
@@ -965,7 +1240,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="37"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
@@ -999,7 +1274,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1035,7 +1310,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1107,7 +1382,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1141,7 +1416,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1177,7 +1452,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1187,188 +1462,6 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="10">
-        <v>2</v>
-      </c>
-      <c r="C12" s="11">
-        <v>2</v>
-      </c>
-      <c r="D12" s="11">
-        <v>2</v>
-      </c>
-      <c r="E12" s="11">
-        <v>2</v>
-      </c>
-      <c r="F12" s="11">
-        <v>2</v>
-      </c>
-      <c r="G12" s="11">
-        <v>1</v>
-      </c>
-      <c r="H12" s="11">
-        <v>1</v>
-      </c>
-      <c r="I12" s="11">
-        <v>1</v>
-      </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="37"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="17">
-        <v>4</v>
-      </c>
-      <c r="C13" s="7">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2</v>
-      </c>
-      <c r="E13" s="7">
-        <v>4</v>
-      </c>
-      <c r="F13" s="7">
-        <v>3</v>
-      </c>
-      <c r="G13" s="7">
-        <v>2</v>
-      </c>
-      <c r="H13" s="7">
-        <v>3</v>
-      </c>
-      <c r="I13" s="7">
-        <v>3</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="30">
-        <f>SUMPRODUCT(B13:I13, $B$2:$I$2)</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="17">
-        <v>2</v>
-      </c>
-      <c r="C14" s="7">
-        <v>3</v>
-      </c>
-      <c r="D14" s="7">
-        <v>3</v>
-      </c>
-      <c r="E14" s="7">
-        <v>3</v>
-      </c>
-      <c r="F14" s="7">
-        <v>3</v>
-      </c>
-      <c r="G14" s="7">
-        <v>3</v>
-      </c>
-      <c r="H14" s="7">
-        <v>4</v>
-      </c>
-      <c r="I14" s="7">
-        <v>3</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="30">
-        <f>SUMPRODUCT(B14:I14, $B$2:$I$2)</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="18">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8">
-        <v>3</v>
-      </c>
-      <c r="D15" s="8">
-        <v>4</v>
-      </c>
-      <c r="E15" s="8">
-        <v>3</v>
-      </c>
-      <c r="F15" s="8">
-        <v>3</v>
-      </c>
-      <c r="G15" s="8">
-        <v>3</v>
-      </c>
-      <c r="H15" s="8">
-        <v>3</v>
-      </c>
-      <c r="I15" s="8">
-        <v>4</v>
-      </c>
-      <c r="J15" s="39"/>
-      <c r="K15" s="40">
-        <f>SUMPRODUCT(B15:I15, $B$2:$I$2)</f>
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1376,6 +1469,667 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11">
+        <v>2</v>
+      </c>
+      <c r="F2" s="11">
+        <v>2</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="37"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
+      <c r="H3" s="7">
+        <v>3</v>
+      </c>
+      <c r="I3" s="7">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="30">
+        <f>SUMPRODUCT(B3:I3, Notation1!$B$2:$I$2)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4</v>
+      </c>
+      <c r="I4" s="7">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="30">
+        <f>SUMPRODUCT(B4:I4, Notation1!$B$2:$I$2)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8">
+        <v>3</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3</v>
+      </c>
+      <c r="H5" s="8">
+        <v>3</v>
+      </c>
+      <c r="I5" s="8">
+        <v>4</v>
+      </c>
+      <c r="J5" s="39"/>
+      <c r="K5" s="40">
+        <f>SUMPRODUCT(B5:I5, Notation1!$B$2:$I$2)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="47"/>
+      <c r="G11" s="52"/>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="52"/>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="47"/>
+      <c r="G13" s="52"/>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="47"/>
+      <c r="G14" s="52"/>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="47"/>
+      <c r="G15" s="52"/>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="52"/>
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="47"/>
+      <c r="G17" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="52"/>
+      <c r="K18" s="23"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="52"/>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="47"/>
+      <c r="G20" s="52"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="52"/>
+      <c r="K21" s="23"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="52"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="55"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="58"/>
+      <c r="B27" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
@@ -1481,7 +2235,7 @@
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="30">
-        <f>SUMPRODUCT(B3:I3, $B$2:$I$2)</f>
+        <f t="shared" ref="K3:K8" si="0">SUMPRODUCT(B3:I3, $B$2:$I$2)</f>
         <v>52</v>
       </c>
     </row>
@@ -1515,7 +2269,7 @@
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="30">
-        <f>SUMPRODUCT(B4:I4, $B$2:$I$2)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
@@ -1549,7 +2303,7 @@
       </c>
       <c r="J5" s="27"/>
       <c r="K5" s="28">
-        <f>SUMPRODUCT(B5:I5, $B$2:$I$2)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
@@ -1585,7 +2339,7 @@
         <v>18</v>
       </c>
       <c r="K6" s="31">
-        <f>SUMPRODUCT(B6:I6, $B$2:$I$2)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
@@ -1619,7 +2373,7 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="30">
-        <f>SUMPRODUCT(B7:I7, $B$2:$I$2)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
@@ -1655,7 +2409,7 @@
         <v>19</v>
       </c>
       <c r="K8" s="29">
-        <f>SUMPRODUCT(B8:I8, $B$2:$I$2)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>

</xml_diff>